<commit_message>
Removed unnecessary testing files; changed some header definitions
</commit_message>
<xml_diff>
--- a/e2e/testing-files/Height_0_20198281030_QTOF_small.xlsx
+++ b/e2e/testing-files/Height_0_20198281030_QTOF_small.xlsx
@@ -103,10 +103,10 @@
     <t xml:space="preserve">Spectrum reference file name</t>
   </si>
   <si>
-    <t xml:space="preserve">MS1 isotopic spectrum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MS/MS spectrum</t>
+    <t xml:space="preserve">MS1 spectrum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MSMS spectrum</t>
   </si>
   <si>
     <t xml:space="preserve">POS_001_BLANK01</t>
@@ -570,8 +570,8 @@
   </sheetPr>
   <dimension ref="A1:DB4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="DB5" activeCellId="0" sqref="DB5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="T1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AB1" activeCellId="0" sqref="AB1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>